<commit_message>
Just adding finishing touches
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodolfo\Desktop\microBiltProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC11D6A0-596D-4EF1-BFE2-2D48469973CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BF77A-0C5A-4D48-907B-9350D7B80B88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13824" yWindow="1644" windowWidth="9216" windowHeight="6156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -44,6 +44,60 @@
   </si>
   <si>
     <t>At 3003 COOL RIDGE CV since Thu Jul 07 2016 00:00:00 GMT-0400 (Eastern Daylight Time)</t>
+  </si>
+  <si>
+    <t>Michelle Semexant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4233836550 6786434050 6786434050 6783349534 6786434050 7708743159 7709891035 7709891035 6783343495 6783349534 6783349534 7707329164 6786434050 </t>
+  </si>
+  <si>
+    <t>At 2731 VALLEY GREEN DR from Thu Mar 21 2019 to Tue Aug 13 2019</t>
+  </si>
+  <si>
+    <t>Henry Turner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2158372470 4047290980 6786343071 6789061865 8505904243 2085202431 6264754955 8502944299 8502944299 8502944299 8503850412 4042540441 4045561004 8503052955 8506560525 </t>
+  </si>
+  <si>
+    <t>At 515 ROSEDOWN WAY since Thu Oct 05 2017</t>
+  </si>
+  <si>
+    <t>Jason Hyman</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 1974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4042293909 4046643327 4048738310 4048738310 6783586414 4042550808 4042550808 4043925135 4043925135 6783586414 6783586414 6785954385 6785954386 7709771941 5124979968 4046643327 </t>
+  </si>
+  <si>
+    <t>At 590 BRIDGEWATER DR since Mon Jul 02 2012</t>
+  </si>
+  <si>
+    <t>David Earley</t>
+  </si>
+  <si>
+    <t>Sat Oct 28 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4436945686 4436943766 5087985592 5087985592 7635444403 6123452837 6126707125 6129913083 7634584476 2147558136 2147558136 2147558136 </t>
+  </si>
+  <si>
+    <t>At 5147 WELLSLEY BND from Sat Apr 02 2016 to Sun Nov 04 2018</t>
+  </si>
+  <si>
+    <t>Curran Sullivan</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8053251450 8053251036 8053251450 8057322769 8649334047 8053251450 8056887004 8056887004 8056889053 8057322769 8053251036 8053251037 </t>
+  </si>
+  <si>
+    <t>At 2309 FORREST WALK since Mon Aug 12 2019</t>
   </si>
 </sst>
 </file>
@@ -79,9 +133,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,16 +449,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.09765625" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="76.796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -448,7 +502,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>35418</v>
       </c>
       <c r="D3">
@@ -456,12 +510,97 @@
       </c>
       <c r="E3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>32287</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>30923</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E6 A8:E8 A7:D7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>